<commit_message>
include color in text analysis
</commit_message>
<xml_diff>
--- a/data/category_mapping.xlsx
+++ b/data/category_mapping.xlsx
@@ -8,30 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanorduz/Documents/codinsky_reply/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B1B629-8730-1D43-84E3-F9C6FCC3FCBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCB6A60-FB76-6847-987C-BB97B43A0026}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="2580" windowWidth="27640" windowHeight="16940" xr2:uid="{165EBEFB-B499-3345-B605-2424EC5F55D1}"/>
+    <workbookView xWindow="1120" yWindow="1560" windowWidth="27640" windowHeight="16940" xr2:uid="{165EBEFB-B499-3345-B605-2424EC5F55D1}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Style</t>
   </si>
@@ -51,36 +45,6 @@
     <t xml:space="preserve">pleasant </t>
   </si>
   <si>
-    <t xml:space="preserve">trust,  charm, helpful, talented, clear </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ok, fine, confident, reliable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">energetic, adventurous, magnificent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">challenging, though, stange, unusual </t>
-  </si>
-  <si>
-    <t xml:space="preserve">adorable, love, ideal, beautiful, considerate, glamorous, bright, fantastic </t>
-  </si>
-  <si>
-    <t xml:space="preserve">young, rapid, quick, modern, joy, cheerfulness, brave </t>
-  </si>
-  <si>
-    <t>imaginative, success, important, encouraged, enthusiatic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">old, ancient, awful, angry, depressed, disgusted, embarrassed </t>
-  </si>
-  <si>
-    <t>moody, clumsy , late, slow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aggressive, annoying, ashamed, bored, defeated, dizzy </t>
-  </si>
-  <si>
     <t xml:space="preserve">square </t>
   </si>
   <si>
@@ -108,24 +72,12 @@
     <t>Keywords</t>
   </si>
   <si>
-    <t>fear, timid, confused, frightened , aggressive</t>
-  </si>
-  <si>
-    <t>circle</t>
-  </si>
-  <si>
-    <t>rectangular</t>
-  </si>
-  <si>
     <t>line</t>
   </si>
   <si>
     <t>angle</t>
   </si>
   <si>
-    <t>oval</t>
-  </si>
-  <si>
     <t>half circle</t>
   </si>
   <si>
@@ -135,17 +87,92 @@
     <t>triangle</t>
   </si>
   <si>
-    <t>background color</t>
-  </si>
-  <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adorable, love, ideal, beautiful, considerate, glamorous, bright, fantastic, magnificent,  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">imaginative, success, important, encouraged, enthusiatic, different, gain, learn, learned, precious, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fear, timid, confused, frightened , aggressive, tired, sleepy, anxiety, worry, worried, heavy, ill, sick, unhappy, scared, uncontrolable, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aggressive, annoying, ashamed, bored, defeated, dizzy, tired, exhausted, done, vulnerable, unforgiving, rage, dull, sleepless, late, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">young, rapid, quick, modern, joy, cheerfulness, brave, happy, fond, cheers, relieved, relief, flattered, fullfiling, delight, genial, gracious, joyous, jolly, </t>
+  </si>
+  <si>
+    <t>bezier curve</t>
+  </si>
+  <si>
+    <t>circle donut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trust,  charm, helpful, talented, clear, romantic, attracted, attractive, intimidate, mourn, enrich, generous, dazzling, holy, pure, fundamental, trivial, truth, true, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">challenging, though, strange, unusual, bizzare, odd, abnormal, betrayed, trivial, false, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">old, ancient, awful, angry, depressed, disgusted, embarrassed, rage, unforgiving, regret, sick, melancholy, weep, cry, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">moody, clumsy , late, slow, weird, sleepy, depressed, lonely, confront, mellow, boring, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok, fine, confident, reliable, doing well, well, meh, usual, yawn, sincere, warm, moderate, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">energetic, adventurous, magnificent, excited, delirious, euphoria, super, going out, desire, desire, happy, charm, lucky, content, miss, saudade, mega, uber, thrill, dramatic, breathtaking, astonishing, interesting, intrigue, very, over, power, moving, wild, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">oval, paralel line, </t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>circle, vertex</t>
+  </si>
+  <si>
+    <t>227, 66, 52, 89</t>
+  </si>
+  <si>
+    <t>72, 35, 80, 31</t>
+  </si>
+  <si>
+    <t>138, 115, 159, 62</t>
+  </si>
+  <si>
+    <t>52, 0, 21, 20</t>
+  </si>
+  <si>
+    <t>128, 182, 211, 83</t>
+  </si>
+  <si>
+    <t>86, 130, 162, 64</t>
+  </si>
+  <si>
+    <t>27, 54, 138, 54</t>
+  </si>
+  <si>
+    <t>183, 189, 214, 84</t>
+  </si>
+  <si>
+    <t>168, 177, 128, 69</t>
+  </si>
+  <si>
+    <t>234, 193, 55, 92</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +187,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,9 +215,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BEA636-2B0C-8E4F-B228-6ABE593DD227}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -510,138 +544,175 @@
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="61.5" customWidth="1"/>
     <col min="3" max="3" width="41.5" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>18</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>